<commit_message>
fix hps field 41 - 7 - 48
</commit_message>
<xml_diff>
--- a/File/Fields_MISR_HPS.xlsx
+++ b/File/Fields_MISR_HPS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="119">
   <si>
     <t xml:space="preserve">Secondary bit map </t>
   </si>
@@ -285,6 +285,102 @@
   </si>
   <si>
     <t>field_length</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Value_error</t>
+  </si>
+  <si>
+    <t>0000000000000000</t>
+  </si>
+  <si>
+    <t>303030303030</t>
+  </si>
+  <si>
+    <t>34373134343539393633323439393330</t>
+  </si>
+  <si>
+    <t>303030303030303031303030</t>
+  </si>
+  <si>
+    <t>31383037323230313331</t>
+  </si>
+  <si>
+    <t>303030303836</t>
+  </si>
+  <si>
+    <t>313830373232303133313431</t>
+  </si>
+  <si>
+    <t>31373132</t>
+  </si>
+  <si>
+    <t>30373232</t>
+  </si>
+  <si>
+    <t>383130313031353130313463</t>
+  </si>
+  <si>
+    <t>303030</t>
+  </si>
+  <si>
+    <t>323030</t>
+  </si>
+  <si>
+    <t>34383134</t>
+  </si>
+  <si>
+    <t>303131323030</t>
+  </si>
+  <si>
+    <t>3030303030303030</t>
+  </si>
+  <si>
+    <t>3437313434353939363332343939333044313731323232363130303030323636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38 31 38 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 32 33 30 31 37 36 34 30 30 34 37 34 30 30 </t>
+  </si>
+  <si>
+    <t>30 30 34 37 34 30 30 30 31 30 30 35 20 20 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 31 32 33 34 35 36 37 38 45 47 59 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 38 50 31 30 30 33 32 41 35 35 34 41 39 36 34 35 39 45 33 36 38 42 46 36 30 42 39 32 37 45 39 46 34 41 44 31 34 45 39 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 20 20 20 20 20 20 20 </t>
+  </si>
+  <si>
+    <t>09 30 31 30 31 30 30 30 30 30</t>
+  </si>
+  <si>
+    <t>1 35 5F 2A 02 08 40 5F 34 01 00 82 02 7C 00 84 07 A0 00 00 00 03 10 10 95 05 08 40 24 00 00 9A 03 18 07 22 9C 01 00 9F 02 06 00 00 00 00 10 00 9F 03 06 00 00 00 00 00 00 9F 09 02 00 8C 9F 10 07 06 01 0A 03 A0 E0 04 9F 1A 02 08 40 9F 1E 08 32 4B 36 32 34 34 37 37 9F 26 08 A4 94 C1 42 54 B7 78 60 9F 27 01 80 9F 33 03 E0 F0 C8 9F 34 03 42 03 00 9F 35 01 22 9F 36 02 00 AC 9F 37 04 AF 0E C5 FA 9F 41 03 00 00 86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 25 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 30 </t>
+  </si>
+  <si>
+    <t>00 00 00 00 00 00 00 00</t>
+  </si>
+  <si>
+    <t>in HPS doc 8 byte and in image 16 byte</t>
+  </si>
+  <si>
+    <t>Error_message</t>
   </si>
 </sst>
 </file>
@@ -312,12 +408,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -332,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -341,12 +443,52 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -621,19 +763,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="4"/>
+    <col min="7" max="7" width="31" style="9" customWidth="1"/>
+    <col min="8" max="8" width="33.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -646,8 +791,20 @@
       <c r="D1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -660,8 +817,17 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -674,8 +840,17 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4">
+        <v>53</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -688,8 +863,17 @@
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -702,8 +886,17 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4">
+        <v>10</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -716,8 +909,14 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -730,8 +929,17 @@
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -744,8 +952,17 @@
       <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>10</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -758,8 +975,17 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -772,8 +998,17 @@
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4">
+        <v>10</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -786,8 +1021,14 @@
       <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -800,8 +1041,17 @@
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4">
+        <v>10</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -814,8 +1064,17 @@
       <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" s="4">
+        <v>30</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -828,8 +1087,17 @@
       <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4">
+        <v>10</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -842,8 +1110,17 @@
       <c r="D15" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4">
+        <v>10</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -856,8 +1133,14 @@
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -870,8 +1153,17 @@
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4">
+        <v>10</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -884,8 +1176,17 @@
       <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4">
+        <v>53</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -898,8 +1199,17 @@
       <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>28</v>
+      </c>
+      <c r="F19" s="4">
+        <v>53</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -912,8 +1222,17 @@
       <c r="D20" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>37</v>
+      </c>
+      <c r="F20" s="4">
+        <v>53</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -926,8 +1245,14 @@
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -940,8 +1265,14 @@
       <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -954,8 +1285,14 @@
       <c r="D23" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -968,8 +1305,17 @@
       <c r="D24" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24" s="4">
+        <v>30</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -982,8 +1328,17 @@
       <c r="D25" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25" s="4">
+        <v>30</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -996,8 +1351,17 @@
       <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>99</v>
+      </c>
+      <c r="F26" s="4">
+        <v>53</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1010,8 +1374,14 @@
       <c r="D27" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>999</v>
+      </c>
+      <c r="F27" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1024,8 +1394,17 @@
       <c r="D28" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>999</v>
+      </c>
+      <c r="F28" s="4">
+        <v>63</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1038,8 +1417,17 @@
       <c r="D29" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29" s="4">
+        <v>10</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1052,36 +1440,63 @@
       <c r="D30" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="5">
         <v>52</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="E31" s="5">
+        <v>8</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="5">
         <v>53</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E32" s="5">
+        <v>18</v>
+      </c>
+      <c r="F32" s="8">
+        <v>53</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1094,22 +1509,37 @@
       <c r="D33" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="E33">
+        <v>120</v>
+      </c>
+      <c r="F33" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="5">
         <v>55</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E34" s="5">
+        <v>255</v>
+      </c>
+      <c r="F34" s="8">
+        <v>63</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1122,8 +1552,14 @@
       <c r="D35" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>45</v>
+      </c>
+      <c r="F35" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1136,36 +1572,60 @@
       <c r="D36" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="E36">
+        <v>999</v>
+      </c>
+      <c r="F36" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="5">
         <v>63</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="E37" s="5">
+        <v>999</v>
+      </c>
+      <c r="F37" s="8">
+        <v>63</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="5">
         <v>64</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="5">
+        <v>8</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1178,8 +1638,14 @@
       <c r="D39" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1192,8 +1658,14 @@
       <c r="D40" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>999</v>
+      </c>
+      <c r="F40" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1206,8 +1678,14 @@
       <c r="D41" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1220,8 +1698,14 @@
       <c r="D42" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>10</v>
+      </c>
+      <c r="F42" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1234,8 +1718,14 @@
       <c r="D43" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1248,8 +1738,14 @@
       <c r="D44" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>10</v>
+      </c>
+      <c r="F44" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1262,8 +1758,14 @@
       <c r="D45" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>10</v>
+      </c>
+      <c r="F45" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1276,8 +1778,14 @@
       <c r="D46" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1290,8 +1798,14 @@
       <c r="D47" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>10</v>
+      </c>
+      <c r="F47" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1304,8 +1818,14 @@
       <c r="D48" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>10</v>
+      </c>
+      <c r="F48" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1318,8 +1838,14 @@
       <c r="D49" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>16</v>
+      </c>
+      <c r="F49" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1332,8 +1858,14 @@
       <c r="D50" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>16</v>
+      </c>
+      <c r="F50" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1346,8 +1878,14 @@
       <c r="D51" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>16</v>
+      </c>
+      <c r="F51" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1360,8 +1898,14 @@
       <c r="D52" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>16</v>
+      </c>
+      <c r="F52" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1374,8 +1918,14 @@
       <c r="D53" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>17</v>
+      </c>
+      <c r="F53" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1388,8 +1938,14 @@
       <c r="D54" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>999</v>
+      </c>
+      <c r="F54" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1401,6 +1957,12 @@
       </c>
       <c r="D55" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add time with RtcGetMW for ASCII
</commit_message>
<xml_diff>
--- a/File/Fields_MISR_HPS.xlsx
+++ b/File/Fields_MISR_HPS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="120">
   <si>
     <t xml:space="preserve">Secondary bit map </t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>Error_message</t>
+  </si>
+  <si>
+    <t>Server_length</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +421,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -452,9 +467,17 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -776,9 +799,11 @@
     <col min="6" max="6" width="9" style="4"/>
     <col min="7" max="7" width="31" style="9" customWidth="1"/>
     <col min="8" max="8" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -803,8 +828,20 @@
       <c r="H1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -826,8 +863,18 @@
       <c r="G2" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>64</v>
+      </c>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -849,8 +896,20 @@
       <c r="G3" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>19</v>
+      </c>
+      <c r="K3" s="12">
+        <v>16</v>
+      </c>
+      <c r="L3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -872,8 +931,20 @@
       <c r="G4" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4" s="12">
+        <v>6</v>
+      </c>
+      <c r="L4" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -895,8 +966,20 @@
       <c r="G5" s="9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>12</v>
+      </c>
+      <c r="K5" s="12">
+        <v>12</v>
+      </c>
+      <c r="L5" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -915,8 +998,18 @@
       <c r="F6" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -938,8 +1031,20 @@
       <c r="G7" s="9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7" s="12">
+        <v>10</v>
+      </c>
+      <c r="L7" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -961,8 +1066,20 @@
       <c r="G8" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8" s="12">
+        <v>6</v>
+      </c>
+      <c r="L8" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -984,8 +1101,20 @@
       <c r="G9" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9" s="12">
+        <v>12</v>
+      </c>
+      <c r="L9" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1007,8 +1136,20 @@
       <c r="G10" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10" s="12">
+        <v>4</v>
+      </c>
+      <c r="L10" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1027,8 +1168,18 @@
       <c r="F11" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1050,8 +1201,20 @@
       <c r="G12" s="9" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12" s="12">
+        <v>4</v>
+      </c>
+      <c r="L12" s="12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1073,8 +1236,20 @@
       <c r="G13" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13" s="12">
+        <v>12</v>
+      </c>
+      <c r="L13" s="12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1096,8 +1271,20 @@
       <c r="G14" s="9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14" s="12">
+        <v>3</v>
+      </c>
+      <c r="L14" s="12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1119,8 +1306,20 @@
       <c r="G15" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15" s="12">
+        <v>3</v>
+      </c>
+      <c r="L15" s="12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1139,8 +1338,18 @@
       <c r="F16" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1162,8 +1371,20 @@
       <c r="G17" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17" s="12">
+        <v>4</v>
+      </c>
+      <c r="L17" s="12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1185,8 +1406,20 @@
       <c r="G18" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18" s="12">
+        <v>6</v>
+      </c>
+      <c r="L18" s="12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1208,8 +1441,20 @@
       <c r="G19" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19">
+        <v>28</v>
+      </c>
+      <c r="K19" s="12">
+        <v>8</v>
+      </c>
+      <c r="L19" s="12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1231,8 +1476,20 @@
       <c r="G20" s="9" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20">
+        <v>37</v>
+      </c>
+      <c r="K20" s="12">
+        <v>36</v>
+      </c>
+      <c r="L20" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1251,8 +1508,17 @@
       <c r="F21" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21">
+        <v>12</v>
+      </c>
+      <c r="L21">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1271,8 +1537,17 @@
       <c r="F22" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1291,8 +1566,17 @@
       <c r="F23" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1314,8 +1598,20 @@
       <c r="G24" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="5">
+        <v>15</v>
+      </c>
+      <c r="K24" s="5">
+        <v>8</v>
+      </c>
+      <c r="L24" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1337,8 +1633,20 @@
       <c r="G25" s="9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="13">
+        <v>15</v>
+      </c>
+      <c r="K25" s="13">
+        <v>15</v>
+      </c>
+      <c r="L25" s="13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1360,8 +1668,20 @@
       <c r="G26" s="9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="5">
+        <v>99</v>
+      </c>
+      <c r="K26" s="5">
+        <v>11</v>
+      </c>
+      <c r="L26" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1380,8 +1700,17 @@
       <c r="F27" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27">
+        <v>999</v>
+      </c>
+      <c r="L27">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="57" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1403,8 +1732,20 @@
       <c r="G28" s="9" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" s="5">
+        <v>999</v>
+      </c>
+      <c r="K28" s="5">
+        <v>936</v>
+      </c>
+      <c r="L28" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1426,8 +1767,20 @@
       <c r="G29" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1446,8 +1799,17 @@
       <c r="F30" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1472,8 +1834,20 @@
       <c r="H31" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="5">
+        <v>8</v>
+      </c>
+      <c r="K31" s="5">
+        <v>16</v>
+      </c>
+      <c r="L31" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1495,8 +1869,17 @@
       <c r="G32" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" s="5">
+        <v>18</v>
+      </c>
+      <c r="L32" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1515,8 +1898,17 @@
       <c r="F33" s="4">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33">
+        <v>120</v>
+      </c>
+      <c r="L33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="5" customFormat="1" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1538,8 +1930,17 @@
       <c r="G34" s="10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J34" s="5">
+        <v>255</v>
+      </c>
+      <c r="L34" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1558,8 +1959,17 @@
       <c r="F35" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35">
+        <v>45</v>
+      </c>
+      <c r="L35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1578,8 +1988,17 @@
       <c r="F36" s="4">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36">
+        <v>999</v>
+      </c>
+      <c r="L36">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1601,8 +2020,17 @@
       <c r="G37" s="10" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I37" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" s="5">
+        <v>999</v>
+      </c>
+      <c r="L37" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1624,8 +2052,17 @@
       <c r="G38" s="10" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="5">
+        <v>8</v>
+      </c>
+      <c r="L38" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1644,8 +2081,17 @@
       <c r="F39" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J39">
+        <v>8</v>
+      </c>
+      <c r="L39">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1664,8 +2110,17 @@
       <c r="F40" s="4">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J40">
+        <v>999</v>
+      </c>
+      <c r="L40">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1684,8 +2139,17 @@
       <c r="F41" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I41" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J41">
+        <v>6</v>
+      </c>
+      <c r="L41">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1704,8 +2168,17 @@
       <c r="F42" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J42">
+        <v>10</v>
+      </c>
+      <c r="L42">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1724,8 +2197,17 @@
       <c r="F43" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J43">
+        <v>10</v>
+      </c>
+      <c r="L43">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1744,8 +2226,17 @@
       <c r="F44" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I44" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44">
+        <v>10</v>
+      </c>
+      <c r="L44">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1764,8 +2255,17 @@
       <c r="F45" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J45">
+        <v>10</v>
+      </c>
+      <c r="L45">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1784,8 +2284,17 @@
       <c r="F46" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I46" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J46">
+        <v>10</v>
+      </c>
+      <c r="L46">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1804,8 +2313,17 @@
       <c r="F47" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J47">
+        <v>10</v>
+      </c>
+      <c r="L47">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1824,8 +2342,17 @@
       <c r="F48" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J48">
+        <v>10</v>
+      </c>
+      <c r="L48">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1844,8 +2371,17 @@
       <c r="F49" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J49">
+        <v>16</v>
+      </c>
+      <c r="L49">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1864,8 +2400,17 @@
       <c r="F50" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J50">
+        <v>16</v>
+      </c>
+      <c r="L50">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1884,8 +2429,17 @@
       <c r="F51" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I51" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J51">
+        <v>16</v>
+      </c>
+      <c r="L51">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1904,8 +2458,17 @@
       <c r="F52" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I52" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J52">
+        <v>16</v>
+      </c>
+      <c r="L52">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1924,8 +2487,17 @@
       <c r="F53" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I53" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J53">
+        <v>17</v>
+      </c>
+      <c r="L53">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1944,8 +2516,17 @@
       <c r="F54" s="4">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="I54" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J54">
+        <v>999</v>
+      </c>
+      <c r="L54">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1963,6 +2544,15 @@
       </c>
       <c r="F55" s="4" t="s">
         <v>87</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J55">
+        <v>8</v>
+      </c>
+      <c r="L55">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>